<commit_message>
CP03ISSP Cal Sheet changes
1. Changed Lat Lon format on Moorings tab
2. Changed reference designators to reflect what is in Instrument
Availability worksheet rev 1-09
3. Deleted templates
</commit_message>
<xml_diff>
--- a/CP03ISSP/Omaha_Cal_Info_CP03ISSP_00001.xlsx
+++ b/CP03ISSP/Omaha_Cal_Info_CP03ISSP_00001.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5860" yWindow="9580" windowWidth="31300" windowHeight="12060" tabRatio="579"/>
+    <workbookView xWindow="5865" yWindow="9585" windowWidth="29040" windowHeight="12060" tabRatio="579" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="101">
   <si>
     <t>Ref Des</t>
   </si>
@@ -232,12 +232,6 @@
     <t>Mooring Serial Number</t>
   </si>
   <si>
-    <t>SheetRef:acs137_calData_CC_taarray</t>
-  </si>
-  <si>
-    <t>SheetRef:acs137_calData_CC_tcarray</t>
-  </si>
-  <si>
     <t>Constant.  wllower = Lower wavelength limit for spectra fit. From DPS: 217 nm (1-cm pathlength probe tip) or 220 nm (4-cm pathlength probe tip)</t>
   </si>
   <si>
@@ -250,28 +244,13 @@
     <t>CP03ISSP-00001</t>
   </si>
   <si>
-    <t>CP03ISSP-SP001-02-DOSTAJ000</t>
-  </si>
-  <si>
     <t>Requires TEMPWAT, PRESWAT and PRACSAL from CP03ISSP-SP001-09-CTDPFJ000</t>
-  </si>
-  <si>
-    <t>CP03ISSP-SP001-04-OPTAAJ000</t>
   </si>
   <si>
     <t>CP03ISSP-SP001-05-VELPTJ000</t>
   </si>
   <si>
-    <t>CP03ISSP-SP001-06-NUTNRJ000</t>
-  </si>
-  <si>
     <t>CP03ISSP-SP001-07-SPKIRJ000</t>
-  </si>
-  <si>
-    <t>CP03ISSP-SP001-08-FLORTJ000</t>
-  </si>
-  <si>
-    <t>CP03ISSP-SP001-09-CTDPFJ000</t>
   </si>
   <si>
     <t>CP03ISSP-SP001-10-PARADJ000</t>
@@ -327,18 +306,45 @@
   <si>
     <t>ACS-145 data is not correct -- pending extraction from the vendor provided files</t>
   </si>
+  <si>
+    <t>70° 53.3000'W</t>
+  </si>
+  <si>
+    <t>40° 21.8833'N</t>
+  </si>
+  <si>
+    <t>SheetRef:acs145_calData_CC_taarray</t>
+  </si>
+  <si>
+    <t>SheetRef:acs145_calData_CC_tcarray</t>
+  </si>
+  <si>
+    <t>CP03ISSP-SP001-06-DOSTAJ000</t>
+  </si>
+  <si>
+    <t>CP03ISSP-SP001-02-OPTAAJ000</t>
+  </si>
+  <si>
+    <t>CP03ISSP-SP001-03-NUTNRJ000</t>
+  </si>
+  <si>
+    <t>CP03ISSP-SP001-09-FLORTJ000</t>
+  </si>
+  <si>
+    <t>CP03ISSP-SP001-08-CTDPFJ000</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="168" formatCode="0.000E+00"/>
-    <numFmt numFmtId="169" formatCode="0.00000"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="0.000E+00"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="35" x14ac:knownFonts="1">
     <font>
@@ -673,14 +679,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
@@ -1226,7 +1232,7 @@
     <xf numFmtId="14" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1256,10 +1262,10 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1286,7 +1292,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="20" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="15" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1297,10 +1303,10 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1850,7 +1856,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Read Me"/>
@@ -2190,28 +2196,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" customWidth="1"/>
-    <col min="11" max="11" width="57.1640625" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" customWidth="1"/>
+    <col min="11" max="11" width="57.140625" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="12" customFormat="1" ht="28">
+    <row r="1" spans="1:13" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2246,12 +2252,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2265,111 +2271,111 @@
       <c r="F2" s="38">
         <v>42015</v>
       </c>
-      <c r="G2" s="39">
-        <v>40.364766666666668</v>
-      </c>
-      <c r="H2" s="39">
-        <v>-70.888300000000001</v>
+      <c r="G2" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" s="39" t="s">
+        <v>92</v>
       </c>
       <c r="I2" s="39">
         <v>93</v>
       </c>
       <c r="J2" s="39" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="K2" s="39" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="M2" s="16"/>
     </row>
-    <row r="3" spans="1:13" s="20" customFormat="1">
+    <row r="3" spans="1:13" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C3" s="21"/>
       <c r="D3" s="22"/>
       <c r="E3" s="23"/>
       <c r="F3" s="22"/>
     </row>
-    <row r="4" spans="1:13" s="20" customFormat="1">
+    <row r="4" spans="1:13" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C4" s="21"/>
       <c r="D4" s="22"/>
       <c r="E4" s="23"/>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:13" s="20" customFormat="1">
+    <row r="5" spans="1:13" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C5" s="21"/>
       <c r="D5" s="22"/>
       <c r="E5" s="23"/>
       <c r="F5" s="22"/>
     </row>
-    <row r="6" spans="1:13" s="20" customFormat="1">
+    <row r="6" spans="1:13" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C6" s="21"/>
       <c r="D6" s="22"/>
       <c r="E6" s="23"/>
       <c r="F6" s="22"/>
     </row>
-    <row r="7" spans="1:13" s="20" customFormat="1">
+    <row r="7" spans="1:13" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C7" s="21"/>
       <c r="D7" s="22"/>
       <c r="E7" s="23"/>
       <c r="F7" s="22"/>
     </row>
-    <row r="8" spans="1:13" s="20" customFormat="1">
+    <row r="8" spans="1:13" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C8" s="21"/>
       <c r="D8" s="22"/>
       <c r="E8" s="23"/>
       <c r="F8" s="22"/>
     </row>
-    <row r="9" spans="1:13" s="20" customFormat="1">
+    <row r="9" spans="1:13" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C9" s="21"/>
       <c r="D9" s="22"/>
       <c r="E9" s="23"/>
       <c r="F9" s="22"/>
     </row>
-    <row r="10" spans="1:13" s="20" customFormat="1">
+    <row r="10" spans="1:13" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C10" s="21"/>
       <c r="D10" s="22"/>
       <c r="E10" s="23"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:13" s="20" customFormat="1">
+    <row r="11" spans="1:13" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C11" s="21"/>
       <c r="D11" s="22"/>
       <c r="E11" s="23"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:13" s="20" customFormat="1">
+    <row r="12" spans="1:13" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C12" s="21"/>
       <c r="D12" s="22"/>
       <c r="E12" s="23"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:13" s="20" customFormat="1">
+    <row r="13" spans="1:13" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C13" s="21"/>
       <c r="D13" s="22"/>
       <c r="E13" s="23"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:13" s="20" customFormat="1">
+    <row r="14" spans="1:13" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C14" s="21"/>
       <c r="D14" s="22"/>
       <c r="E14" s="23"/>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:13" s="20" customFormat="1">
+    <row r="15" spans="1:13" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C15" s="21"/>
       <c r="D15" s="22"/>
       <c r="E15" s="23"/>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:13" s="20" customFormat="1">
+    <row r="16" spans="1:13" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C16" s="21"/>
       <c r="D16" s="22"/>
       <c r="E16" s="23"/>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="3:6" s="20" customFormat="1">
+    <row r="17" spans="3:6" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C17" s="21"/>
       <c r="D17" s="22"/>
       <c r="E17" s="23"/>
@@ -2390,20 +2396,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="L58" sqref="L58"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="57.33203125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="57.28515625" style="13" customWidth="1"/>
     <col min="7" max="7" width="65" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28">
+    <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2426,15 +2434,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" s="13" customFormat="1">
+    <row r="3" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C3" s="25">
         <v>1</v>
@@ -2452,12 +2460,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="13" customFormat="1">
-      <c r="A4" s="14" t="s">
-        <v>73</v>
+    <row r="4" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>96</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C4" s="29">
         <v>1</v>
@@ -2475,12 +2483,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="13" customFormat="1">
-      <c r="A5" s="14" t="s">
-        <v>73</v>
+    <row r="5" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>96</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C5" s="29">
         <v>1</v>
@@ -2492,31 +2500,31 @@
         <v>6</v>
       </c>
       <c r="F5" s="42" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="13" customFormat="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="27"/>
       <c r="C6" s="29"/>
       <c r="D6" s="31"/>
       <c r="F6" s="31"/>
     </row>
-    <row r="7" spans="1:7" s="13" customFormat="1">
+    <row r="7" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C7" s="25">
         <v>1</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>49</v>
@@ -2525,21 +2533,21 @@
         <v>57</v>
       </c>
       <c r="G7" s="46" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="13" customFormat="1">
-      <c r="A8" s="14" t="s">
-        <v>75</v>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>97</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C8" s="29">
         <v>1</v>
       </c>
       <c r="D8" s="41" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>50</v>
@@ -2549,18 +2557,18 @@
       </c>
       <c r="G8" s="18"/>
     </row>
-    <row r="9" spans="1:7" s="13" customFormat="1">
-      <c r="A9" s="14" t="s">
-        <v>75</v>
+    <row r="9" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>97</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C9" s="29">
         <v>1</v>
       </c>
       <c r="D9" s="41" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>51</v>
@@ -2570,18 +2578,18 @@
       </c>
       <c r="G9" s="18"/>
     </row>
-    <row r="10" spans="1:7" s="13" customFormat="1">
-      <c r="A10" s="14" t="s">
-        <v>75</v>
+    <row r="10" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>97</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C10" s="29">
         <v>1</v>
       </c>
       <c r="D10" s="41" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>54</v>
@@ -2591,39 +2599,39 @@
       </c>
       <c r="G10" s="18"/>
     </row>
-    <row r="11" spans="1:7" s="13" customFormat="1">
-      <c r="A11" s="14" t="s">
-        <v>75</v>
+    <row r="11" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>97</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C11" s="29">
         <v>1</v>
       </c>
       <c r="D11" s="41" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>52</v>
       </c>
       <c r="F11" s="31" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
       <c r="G11" s="18"/>
     </row>
-    <row r="12" spans="1:7" s="13" customFormat="1">
-      <c r="A12" s="14" t="s">
-        <v>75</v>
+    <row r="12" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>97</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C12" s="29">
         <v>1</v>
       </c>
       <c r="D12" s="41" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>53</v>
@@ -2633,18 +2641,18 @@
       </c>
       <c r="G12" s="18"/>
     </row>
-    <row r="13" spans="1:7" s="13" customFormat="1">
-      <c r="A13" s="14" t="s">
-        <v>75</v>
+    <row r="13" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>97</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C13" s="29">
         <v>1</v>
       </c>
       <c r="D13" s="41" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>55</v>
@@ -2654,46 +2662,46 @@
       </c>
       <c r="G13" s="18"/>
     </row>
-    <row r="14" spans="1:7" s="13" customFormat="1">
-      <c r="A14" s="14" t="s">
-        <v>75</v>
+    <row r="14" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>97</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C14" s="29">
         <v>1</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>56</v>
       </c>
       <c r="F14" s="31" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="G14" s="18"/>
     </row>
-    <row r="15" spans="1:7" s="13" customFormat="1">
+    <row r="15" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="27"/>
       <c r="C15" s="29"/>
       <c r="D15" s="31"/>
       <c r="F15" s="31"/>
     </row>
-    <row r="16" spans="1:7" s="13" customFormat="1">
+    <row r="16" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C16" s="25">
         <v>1</v>
       </c>
       <c r="D16" s="42" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>7</v>
@@ -2705,18 +2713,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="13" customFormat="1">
+    <row r="17" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C17" s="29">
         <v>1</v>
       </c>
       <c r="D17" s="42" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>8</v>
@@ -2728,19 +2736,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="13" customFormat="1">
+    <row r="18" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="B18" s="27"/>
       <c r="C18" s="29"/>
       <c r="D18" s="31"/>
       <c r="F18" s="31"/>
     </row>
-    <row r="19" spans="1:7" s="13" customFormat="1">
+    <row r="19" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C19" s="25">
         <v>1</v>
@@ -2755,15 +2763,15 @@
         <v>217</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="13" customFormat="1">
-      <c r="A20" s="14" t="s">
-        <v>77</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>98</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C20" s="29">
         <v>1</v>
@@ -2778,15 +2786,15 @@
         <v>240</v>
       </c>
       <c r="G20" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="27" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="13" customFormat="1">
-      <c r="A21" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21" s="27" t="s">
-        <v>72</v>
       </c>
       <c r="C21" s="29">
         <v>1</v>
@@ -2804,12 +2812,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="13" customFormat="1">
-      <c r="A22" s="14" t="s">
-        <v>77</v>
+    <row r="22" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>98</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C22" s="29">
         <v>1</v>
@@ -2821,18 +2829,18 @@
         <v>41</v>
       </c>
       <c r="F22" s="42" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G22" s="13" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="13" customFormat="1">
-      <c r="A23" s="14" t="s">
-        <v>77</v>
+    <row r="23" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>98</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C23" s="29">
         <v>1</v>
@@ -2844,18 +2852,18 @@
         <v>43</v>
       </c>
       <c r="F23" s="42" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="13" customFormat="1">
-      <c r="A24" s="14" t="s">
-        <v>77</v>
+    <row r="24" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
+        <v>98</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C24" s="29">
         <v>1</v>
@@ -2867,18 +2875,18 @@
         <v>45</v>
       </c>
       <c r="F24" s="42" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G24" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="13" customFormat="1">
-      <c r="A25" s="14" t="s">
-        <v>77</v>
+    <row r="25" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>98</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C25" s="29">
         <v>1</v>
@@ -2890,25 +2898,25 @@
         <v>47</v>
       </c>
       <c r="F25" s="42" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="G25" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="13" customFormat="1">
+    <row r="26" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
       <c r="B26" s="27"/>
       <c r="C26" s="29"/>
       <c r="D26" s="31"/>
       <c r="F26" s="31"/>
     </row>
-    <row r="27" spans="1:7" s="13" customFormat="1">
+    <row r="27" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C27" s="25">
         <v>1</v>
@@ -2920,15 +2928,15 @@
         <v>34</v>
       </c>
       <c r="F27" s="42" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="13" customFormat="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C28" s="29">
         <v>1</v>
@@ -2940,15 +2948,15 @@
         <v>35</v>
       </c>
       <c r="F28" s="42" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="13" customFormat="1">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C29" s="29">
         <v>1</v>
@@ -2960,22 +2968,22 @@
         <v>36</v>
       </c>
       <c r="F29" s="42" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" s="13" customFormat="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
       <c r="B30" s="27"/>
       <c r="C30" s="29"/>
       <c r="D30" s="31"/>
       <c r="F30" s="31"/>
     </row>
-    <row r="31" spans="1:7" s="13" customFormat="1">
+    <row r="31" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C31" s="25">
         <v>1</v>
@@ -2993,12 +3001,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="13" customFormat="1">
-      <c r="A32" s="14" t="s">
-        <v>79</v>
+    <row r="32" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>99</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C32" s="29">
         <v>1</v>
@@ -3016,12 +3024,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="13" customFormat="1">
-      <c r="A33" s="14" t="s">
-        <v>79</v>
+    <row r="33" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
+        <v>99</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C33" s="29">
         <v>1</v>
@@ -3039,12 +3047,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="13" customFormat="1">
-      <c r="A34" s="14" t="s">
-        <v>79</v>
+    <row r="34" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>99</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C34" s="29">
         <v>1</v>
@@ -3062,12 +3070,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="13" customFormat="1">
-      <c r="A35" s="14" t="s">
-        <v>79</v>
+    <row r="35" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>99</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C35" s="29">
         <v>1</v>
@@ -3085,12 +3093,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="13" customFormat="1">
-      <c r="A36" s="14" t="s">
-        <v>79</v>
+    <row r="36" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
+        <v>99</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C36" s="29">
         <v>1</v>
@@ -3108,12 +3116,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="13" customFormat="1">
-      <c r="A37" s="14" t="s">
-        <v>79</v>
+    <row r="37" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="17" t="s">
+        <v>99</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C37" s="29">
         <v>1</v>
@@ -3131,12 +3139,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="13" customFormat="1">
-      <c r="A38" s="14" t="s">
-        <v>79</v>
+    <row r="38" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
+        <v>99</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C38" s="29">
         <v>1</v>
@@ -3154,12 +3162,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="13" customFormat="1">
-      <c r="A39" s="14" t="s">
-        <v>79</v>
+    <row r="39" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="17" t="s">
+        <v>99</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C39" s="29">
         <v>1</v>
@@ -3177,12 +3185,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="13" customFormat="1">
-      <c r="A40" s="14" t="s">
-        <v>79</v>
+    <row r="40" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="17" t="s">
+        <v>99</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C40" s="29">
         <v>1</v>
@@ -3200,25 +3208,25 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="13" customFormat="1">
+    <row r="41" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="14"/>
       <c r="B41" s="27"/>
       <c r="C41" s="29"/>
       <c r="D41" s="31"/>
       <c r="F41" s="31"/>
     </row>
-    <row r="42" spans="1:7" s="13" customFormat="1">
+    <row r="42" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C42" s="25">
         <v>1</v>
       </c>
       <c r="D42" s="42" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E42" s="13" t="s">
         <v>7</v>
@@ -3230,18 +3238,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="13" customFormat="1">
-      <c r="A43" s="14" t="s">
-        <v>80</v>
+    <row r="43" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="17" t="s">
+        <v>100</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C43" s="29">
         <v>1</v>
       </c>
       <c r="D43" s="42" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E43" s="13" t="s">
         <v>8</v>
@@ -3253,19 +3261,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="13" customFormat="1">
+    <row r="44" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17"/>
       <c r="B44" s="27"/>
       <c r="C44" s="29"/>
       <c r="D44" s="31"/>
       <c r="F44" s="31"/>
     </row>
-    <row r="45" spans="1:7" s="13" customFormat="1">
+    <row r="45" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C45" s="25">
         <v>1</v>
@@ -3280,12 +3288,12 @@
         <v>4248</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="13" customFormat="1">
+    <row r="46" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B46" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C46" s="29">
         <v>1</v>
@@ -3300,12 +3308,12 @@
         <v>2587</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="13" customFormat="1">
+    <row r="47" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C47" s="29">
         <v>1</v>
@@ -3320,29 +3328,37 @@
         <v>1.3589</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="24" customFormat="1">
+    <row r="48" spans="1:7" s="24" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C48" s="25"/>
       <c r="F48" s="32"/>
     </row>
-    <row r="49" spans="1:6" s="13" customFormat="1">
+    <row r="49" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="34" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B49" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C49" s="25">
         <v>1</v>
       </c>
       <c r="D49" s="40" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="F49" s="33"/>
     </row>
-    <row r="50" spans="1:6" s="13" customFormat="1"/>
-    <row r="51" spans="1:6" s="13" customFormat="1"/>
-    <row r="52" spans="1:6" s="13" customFormat="1"/>
-    <row r="53" spans="1:6" s="13" customFormat="1"/>
+    <row r="50" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G50"/>
+    </row>
+    <row r="51" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G51"/>
+    </row>
+    <row r="52" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G52"/>
+    </row>
+    <row r="53" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G53"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3359,15 +3375,15 @@
   <dimension ref="A1:AJ85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.5" style="30"/>
+    <col min="1" max="16384" width="11.42578125" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="30">
         <v>4.6008E-2</v>
       </c>
@@ -3477,7 +3493,7 @@
         <v>-1.137E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="30">
         <v>4.2536999999999998E-2</v>
       </c>
@@ -3587,7 +3603,7 @@
         <v>-1.358E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="30">
         <v>4.3115000000000001E-2</v>
       </c>
@@ -3697,7 +3713,7 @@
         <v>-1.5838999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="30">
         <v>4.3878E-2</v>
       </c>
@@ -3807,7 +3823,7 @@
         <v>-1.8959E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="30">
         <v>4.3221000000000002E-2</v>
       </c>
@@ -3917,7 +3933,7 @@
         <v>-2.0358000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="30">
         <v>4.1510999999999999E-2</v>
       </c>
@@ -4027,7 +4043,7 @@
         <v>-1.9682000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="30">
         <v>3.7416999999999999E-2</v>
       </c>
@@ -4137,7 +4153,7 @@
         <v>-1.8426000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="30">
         <v>3.4866000000000001E-2</v>
       </c>
@@ -4247,7 +4263,7 @@
         <v>-1.6534E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="30">
         <v>3.1199999999999999E-2</v>
       </c>
@@ -4357,7 +4373,7 @@
         <v>-1.4978999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="30">
         <v>2.7692999999999999E-2</v>
       </c>
@@ -4467,7 +4483,7 @@
         <v>-1.3599999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:36">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="30">
         <v>2.4787E-2</v>
       </c>
@@ -4577,7 +4593,7 @@
         <v>-1.2409E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:36">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="30">
         <v>2.1585E-2</v>
       </c>
@@ -4687,7 +4703,7 @@
         <v>-1.1106E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:36">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="30">
         <v>1.9362999999999998E-2</v>
       </c>
@@ -4797,7 +4813,7 @@
         <v>-1.0659999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:36">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="30">
         <v>1.7412E-2</v>
       </c>
@@ -4907,7 +4923,7 @@
         <v>-1.0090999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:36">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="30">
         <v>1.5740000000000001E-2</v>
       </c>
@@ -5017,7 +5033,7 @@
         <v>-9.4520000000000003E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:36">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="30">
         <v>1.4527E-2</v>
       </c>
@@ -5127,7 +5143,7 @@
         <v>-9.214E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:36">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="30">
         <v>1.379E-2</v>
       </c>
@@ -5237,7 +5253,7 @@
         <v>-9.1629999999999993E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:36">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="30">
         <v>1.2543E-2</v>
       </c>
@@ -5347,7 +5363,7 @@
         <v>-9.1640000000000003E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:36">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="30">
         <v>1.1979999999999999E-2</v>
       </c>
@@ -5457,7 +5473,7 @@
         <v>-9.2560000000000003E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:36">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="30">
         <v>1.141E-2</v>
       </c>
@@ -5567,7 +5583,7 @@
         <v>-9.3310000000000008E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:36">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="30">
         <v>1.0869999999999999E-2</v>
       </c>
@@ -5677,7 +5693,7 @@
         <v>-9.4339999999999997E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:36">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="30">
         <v>1.0403000000000001E-2</v>
       </c>
@@ -5787,7 +5803,7 @@
         <v>-9.6699999999999998E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:36">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" s="30">
         <v>1.018E-2</v>
       </c>
@@ -5897,7 +5913,7 @@
         <v>-9.9600000000000001E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:36">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" s="30">
         <v>9.5879999999999993E-3</v>
       </c>
@@ -6007,7 +6023,7 @@
         <v>-9.9190000000000007E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:36">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" s="30">
         <v>9.384E-3</v>
       </c>
@@ -6117,7 +6133,7 @@
         <v>-1.0031999999999999E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:36">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" s="30">
         <v>9.025E-3</v>
       </c>
@@ -6227,7 +6243,7 @@
         <v>-9.8969999999999995E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:36">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" s="30">
         <v>8.5540000000000008E-3</v>
       </c>
@@ -6337,7 +6353,7 @@
         <v>-9.5949999999999994E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:36">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" s="30">
         <v>8.3199999999999993E-3</v>
       </c>
@@ -6447,7 +6463,7 @@
         <v>-9.2449999999999997E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:36">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" s="30">
         <v>7.9459999999999999E-3</v>
       </c>
@@ -6557,7 +6573,7 @@
         <v>-8.9110000000000005E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:36">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="30">
         <v>7.5760000000000003E-3</v>
       </c>
@@ -6667,7 +6683,7 @@
         <v>-8.286E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:36">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="30">
         <v>7.5640000000000004E-3</v>
       </c>
@@ -6777,7 +6793,7 @@
         <v>-7.8480000000000008E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:36">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="30">
         <v>7.2570000000000004E-3</v>
       </c>
@@ -6887,7 +6903,7 @@
         <v>-7.273E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:36">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" s="30">
         <v>7.1209999999999997E-3</v>
       </c>
@@ -6997,7 +7013,7 @@
         <v>-6.6730000000000001E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:36">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" s="30">
         <v>7.1009999999999997E-3</v>
       </c>
@@ -7107,7 +7123,7 @@
         <v>-6.0819999999999997E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:36">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="30">
         <v>6.9690000000000004E-3</v>
       </c>
@@ -7217,7 +7233,7 @@
         <v>-5.555E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:36">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36" s="30">
         <v>7.1580000000000003E-3</v>
       </c>
@@ -7327,7 +7343,7 @@
         <v>-5.0730000000000003E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:36">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" s="30">
         <v>7.0470000000000003E-3</v>
       </c>
@@ -7437,7 +7453,7 @@
         <v>-4.6169999999999996E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:36">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38" s="30">
         <v>7.2830000000000004E-3</v>
       </c>
@@ -7547,7 +7563,7 @@
         <v>-4.3220000000000003E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:36">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="30">
         <v>7.0229999999999997E-3</v>
       </c>
@@ -7657,7 +7673,7 @@
         <v>-4.0289999999999996E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:36">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40" s="30">
         <v>6.6090000000000003E-3</v>
       </c>
@@ -7767,7 +7783,7 @@
         <v>-3.7910000000000001E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:36">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41" s="30">
         <v>6.4440000000000001E-3</v>
       </c>
@@ -7877,7 +7893,7 @@
         <v>-3.5990000000000002E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:36">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42" s="30">
         <v>5.9170000000000004E-3</v>
       </c>
@@ -7987,7 +8003,7 @@
         <v>-3.4169999999999999E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:36">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43" s="30">
         <v>1.9090000000000001E-3</v>
       </c>
@@ -8097,7 +8113,7 @@
         <v>-4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:36">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44" s="30">
         <v>1.421E-3</v>
       </c>
@@ -8207,7 +8223,7 @@
         <v>-1.9699999999999999E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:36">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45" s="30">
         <v>1.3699999999999999E-3</v>
       </c>
@@ -8317,7 +8333,7 @@
         <v>6.6000000000000005E-5</v>
       </c>
     </row>
-    <row r="46" spans="1:36">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46" s="30">
         <v>9.7599999999999998E-4</v>
       </c>
@@ -8427,7 +8443,7 @@
         <v>3.4499999999999998E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:36">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47" s="30">
         <v>5.5900000000000004E-4</v>
       </c>
@@ -8537,7 +8553,7 @@
         <v>6.4800000000000003E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:36">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A48" s="30">
         <v>-1.1E-5</v>
       </c>
@@ -8647,7 +8663,7 @@
         <v>1.0020000000000001E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:36">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49" s="30">
         <v>-5.62E-4</v>
       </c>
@@ -8757,7 +8773,7 @@
         <v>1.3500000000000001E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:36">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A50" s="30">
         <v>-1.3389999999999999E-3</v>
       </c>
@@ -8867,7 +8883,7 @@
         <v>1.5380000000000001E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:36">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51" s="30">
         <v>-2.0699999999999998E-3</v>
       </c>
@@ -8977,7 +8993,7 @@
         <v>1.722E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:36">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52" s="30">
         <v>-2.702E-3</v>
       </c>
@@ -9087,7 +9103,7 @@
         <v>1.714E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:36">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53" s="30">
         <v>-2.8639999999999998E-3</v>
       </c>
@@ -9197,7 +9213,7 @@
         <v>1.7279999999999999E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:36">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54" s="30">
         <v>-2.9510000000000001E-3</v>
       </c>
@@ -9307,7 +9323,7 @@
         <v>1.5299999999999999E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:36">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55" s="30">
         <v>-2.8219999999999999E-3</v>
       </c>
@@ -9417,7 +9433,7 @@
         <v>1.3780000000000001E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:36">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56" s="30">
         <v>-2.7550000000000001E-3</v>
       </c>
@@ -9527,7 +9543,7 @@
         <v>1.0640000000000001E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:36">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57" s="30">
         <v>-2.5140000000000002E-3</v>
       </c>
@@ -9637,7 +9653,7 @@
         <v>9.3599999999999998E-4</v>
       </c>
     </row>
-    <row r="58" spans="1:36">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58" s="30">
         <v>-2.2439999999999999E-3</v>
       </c>
@@ -9747,7 +9763,7 @@
         <v>8.25E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:36">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A59" s="30">
         <v>-2.0070000000000001E-3</v>
       </c>
@@ -9857,7 +9873,7 @@
         <v>6.9899999999999997E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:36">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A60" s="30">
         <v>-1.7780000000000001E-3</v>
       </c>
@@ -9967,7 +9983,7 @@
         <v>6.3199999999999997E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:36">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61" s="30">
         <v>-1.655E-3</v>
       </c>
@@ -10077,7 +10093,7 @@
         <v>4.6700000000000002E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:36">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A62" s="30">
         <v>-1.6310000000000001E-3</v>
       </c>
@@ -10187,7 +10203,7 @@
         <v>3.2499999999999999E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:36">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63" s="30">
         <v>-1.5989999999999999E-3</v>
       </c>
@@ -10297,7 +10313,7 @@
         <v>1.93E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:36">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64" s="30">
         <v>-1.493E-3</v>
       </c>
@@ -10407,7 +10423,7 @@
         <v>6.4999999999999994E-5</v>
       </c>
     </row>
-    <row r="65" spans="1:36">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A65" s="30">
         <v>-1.273E-3</v>
       </c>
@@ -10517,7 +10533,7 @@
         <v>-7.4999999999999993E-5</v>
       </c>
     </row>
-    <row r="66" spans="1:36">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A66" s="30">
         <v>-1.0189999999999999E-3</v>
       </c>
@@ -10627,7 +10643,7 @@
         <v>-1.5899999999999999E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:36">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A67" s="30">
         <v>-7.1699999999999997E-4</v>
       </c>
@@ -10737,7 +10753,7 @@
         <v>-1.7000000000000001E-4</v>
       </c>
     </row>
-    <row r="68" spans="1:36">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A68" s="30">
         <v>-1.8E-5</v>
       </c>
@@ -10847,7 +10863,7 @@
         <v>-3.1100000000000002E-4</v>
       </c>
     </row>
-    <row r="69" spans="1:36">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A69" s="30">
         <v>3.28E-4</v>
       </c>
@@ -10957,7 +10973,7 @@
         <v>-5.0299999999999997E-4</v>
       </c>
     </row>
-    <row r="70" spans="1:36">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A70" s="30">
         <v>5.8299999999999997E-4</v>
       </c>
@@ -11067,7 +11083,7 @@
         <v>-6.7100000000000005E-4</v>
       </c>
     </row>
-    <row r="71" spans="1:36">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A71" s="30">
         <v>8.4999999999999995E-4</v>
       </c>
@@ -11177,7 +11193,7 @@
         <v>-9.0499999999999999E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:36">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A72" s="30">
         <v>1.165E-3</v>
       </c>
@@ -11287,7 +11303,7 @@
         <v>-1.168E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:36">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A73" s="30">
         <v>1.469E-3</v>
       </c>
@@ -11397,7 +11413,7 @@
         <v>-1.3760000000000001E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:36">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A74" s="30">
         <v>1.9949999999999998E-3</v>
       </c>
@@ -11507,7 +11523,7 @@
         <v>-1.586E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:36">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A75" s="30">
         <v>2.3739999999999998E-3</v>
       </c>
@@ -11617,7 +11633,7 @@
         <v>-1.663E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:36">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A76" s="30">
         <v>2.3760000000000001E-3</v>
       </c>
@@ -11727,7 +11743,7 @@
         <v>-1.732E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:36">
+    <row r="77" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A77" s="30">
         <v>2.4130000000000002E-3</v>
       </c>
@@ -11837,7 +11853,7 @@
         <v>-1.681E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:36">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A78" s="30">
         <v>2.166E-3</v>
       </c>
@@ -11947,7 +11963,7 @@
         <v>-1.699E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:36">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A79" s="30">
         <v>1.9530000000000001E-3</v>
       </c>
@@ -12057,7 +12073,7 @@
         <v>-1.627E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:36">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A80" s="30">
         <v>1.7539999999999999E-3</v>
       </c>
@@ -12167,7 +12183,7 @@
         <v>-1.565E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:36">
+    <row r="81" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A81" s="30">
         <v>1.653E-3</v>
       </c>
@@ -12277,7 +12293,7 @@
         <v>-1.4779999999999999E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:36">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A82" s="30">
         <v>1.4339999999999999E-3</v>
       </c>
@@ -12387,7 +12403,7 @@
         <v>-1.253E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:36">
+    <row r="83" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A83" s="30">
         <v>1.5529999999999999E-3</v>
       </c>
@@ -12497,7 +12513,7 @@
         <v>-1.103E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:36">
+    <row r="84" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A84" s="30">
         <v>1.704E-3</v>
       </c>
@@ -12607,7 +12623,7 @@
         <v>-8.92E-4</v>
       </c>
     </row>
-    <row r="85" spans="1:36">
+    <row r="85" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A85" s="30">
         <v>1.725E-3</v>
       </c>
@@ -12732,15 +12748,15 @@
   <dimension ref="A1:AJ85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.5" style="30"/>
+    <col min="1" max="16384" width="11.42578125" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="30">
         <v>0.11464299999999999</v>
       </c>
@@ -12850,7 +12866,7 @@
         <v>-5.0855999999999998E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="30">
         <v>0.11143699999999999</v>
       </c>
@@ -12960,7 +12976,7 @@
         <v>-4.8311E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="30">
         <v>0.10566</v>
       </c>
@@ -13070,7 +13086,7 @@
         <v>-4.7612000000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="30">
         <v>0.103315</v>
       </c>
@@ -13180,7 +13196,7 @@
         <v>-4.4401000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="30">
         <v>0.100078</v>
       </c>
@@ -13290,7 +13306,7 @@
         <v>-4.3917999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="30">
         <v>9.7517999999999994E-2</v>
       </c>
@@ -13400,7 +13416,7 @@
         <v>-4.0932999999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="30">
         <v>9.4977000000000006E-2</v>
       </c>
@@ -13510,7 +13526,7 @@
         <v>-3.9729E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="30">
         <v>9.2086000000000001E-2</v>
       </c>
@@ -13620,7 +13636,7 @@
         <v>-3.8157999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="30">
         <v>8.8232000000000005E-2</v>
       </c>
@@ -13730,7 +13746,7 @@
         <v>-3.6015999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="30">
         <v>8.4955000000000003E-2</v>
       </c>
@@ -13840,7 +13856,7 @@
         <v>-3.3876000000000003E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:36">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="30">
         <v>8.2607E-2</v>
       </c>
@@ -13950,7 +13966,7 @@
         <v>-3.2259999999999997E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:36">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="30">
         <v>7.9913999999999999E-2</v>
       </c>
@@ -14060,7 +14076,7 @@
         <v>-3.0206E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:36">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="30">
         <v>7.8973000000000002E-2</v>
       </c>
@@ -14170,7 +14186,7 @@
         <v>-2.8332E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:36">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="30">
         <v>7.6024999999999995E-2</v>
       </c>
@@ -14280,7 +14296,7 @@
         <v>-2.6426000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:36">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="30">
         <v>7.4902999999999997E-2</v>
       </c>
@@ -14390,7 +14406,7 @@
         <v>-2.4596E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:36">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="30">
         <v>7.3431999999999997E-2</v>
       </c>
@@ -14500,7 +14516,7 @@
         <v>-2.2771E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:36">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="30">
         <v>7.2954000000000005E-2</v>
       </c>
@@ -14610,7 +14626,7 @@
         <v>-2.1378000000000001E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:36">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="30">
         <v>7.2392999999999999E-2</v>
       </c>
@@ -14720,7 +14736,7 @@
         <v>-2.0163E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:36">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="30">
         <v>7.1642999999999998E-2</v>
       </c>
@@ -14830,7 +14846,7 @@
         <v>-1.9016999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:36">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="30">
         <v>7.0186999999999999E-2</v>
       </c>
@@ -14940,7 +14956,7 @@
         <v>-1.8008E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:36">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="30">
         <v>6.9302000000000002E-2</v>
       </c>
@@ -15050,7 +15066,7 @@
         <v>-1.7052000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:36">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="30">
         <v>6.8472000000000005E-2</v>
       </c>
@@ -15160,7 +15176,7 @@
         <v>-1.6406E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:36">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" s="30">
         <v>6.7325999999999997E-2</v>
       </c>
@@ -15270,7 +15286,7 @@
         <v>-1.5685000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:36">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" s="30">
         <v>6.6239999999999993E-2</v>
       </c>
@@ -15380,7 +15396,7 @@
         <v>-1.5491E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:36">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" s="30">
         <v>6.5568000000000001E-2</v>
       </c>
@@ -15490,7 +15506,7 @@
         <v>-1.5266999999999999E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:36">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" s="30">
         <v>6.4459000000000002E-2</v>
       </c>
@@ -15600,7 +15616,7 @@
         <v>-1.5446E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:36">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" s="30">
         <v>6.3698000000000005E-2</v>
       </c>
@@ -15710,7 +15726,7 @@
         <v>-1.5762000000000002E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:36">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" s="30">
         <v>6.2205000000000003E-2</v>
       </c>
@@ -15820,7 +15836,7 @@
         <v>-1.5906E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:36">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" s="30">
         <v>6.1772000000000001E-2</v>
       </c>
@@ -15930,7 +15946,7 @@
         <v>-1.6376000000000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:36">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="30">
         <v>6.0983000000000002E-2</v>
       </c>
@@ -16040,7 +16056,7 @@
         <v>-1.6698000000000001E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:36">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="30">
         <v>5.9484000000000002E-2</v>
       </c>
@@ -16150,7 +16166,7 @@
         <v>-1.7065E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:36">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="30">
         <v>5.885E-2</v>
       </c>
@@ -16260,7 +16276,7 @@
         <v>-1.7538000000000002E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:36">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" s="30">
         <v>5.8035000000000003E-2</v>
       </c>
@@ -16370,7 +16386,7 @@
         <v>-1.7956E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:36">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" s="30">
         <v>5.6728000000000001E-2</v>
       </c>
@@ -16480,7 +16496,7 @@
         <v>-1.8258E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:36">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="30">
         <v>5.6006E-2</v>
       </c>
@@ -16590,7 +16606,7 @@
         <v>-1.8557000000000001E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:36">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36" s="30">
         <v>5.4544000000000002E-2</v>
       </c>
@@ -16700,7 +16716,7 @@
         <v>-1.8412999999999999E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:36">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" s="30">
         <v>5.3428000000000003E-2</v>
       </c>
@@ -16810,7 +16826,7 @@
         <v>-1.8096000000000001E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:36">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38" s="30">
         <v>5.2255000000000003E-2</v>
       </c>
@@ -16920,7 +16936,7 @@
         <v>-1.7731E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:36">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="30">
         <v>5.1347999999999998E-2</v>
       </c>
@@ -17030,7 +17046,7 @@
         <v>-1.7405E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:36">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40" s="30">
         <v>5.0941E-2</v>
       </c>
@@ -17140,7 +17156,7 @@
         <v>-1.6965000000000001E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:36">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41" s="30">
         <v>5.0456000000000001E-2</v>
       </c>
@@ -17250,7 +17266,7 @@
         <v>-1.6688000000000001E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:36">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42" s="30">
         <v>4.9521000000000003E-2</v>
       </c>
@@ -17360,7 +17376,7 @@
         <v>-1.6479000000000001E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:36">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43" s="30">
         <v>5.2349E-2</v>
       </c>
@@ -17470,7 +17486,7 @@
         <v>-1.9583E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:36">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44" s="30">
         <v>5.2712000000000002E-2</v>
       </c>
@@ -17580,7 +17596,7 @@
         <v>-1.9982E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:36">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45" s="30">
         <v>5.2965999999999999E-2</v>
       </c>
@@ -17690,7 +17706,7 @@
         <v>-2.0264000000000001E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:36">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46" s="30">
         <v>5.373E-2</v>
       </c>
@@ -17800,7 +17816,7 @@
         <v>-2.0386000000000001E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:36">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47" s="30">
         <v>5.4421999999999998E-2</v>
       </c>
@@ -17910,7 +17926,7 @@
         <v>-2.0745E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:36">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A48" s="30">
         <v>5.5028000000000001E-2</v>
       </c>
@@ -18020,7 +18036,7 @@
         <v>-2.0560999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:36">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49" s="30">
         <v>5.5216000000000001E-2</v>
       </c>
@@ -18130,7 +18146,7 @@
         <v>-2.0379999999999999E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:36">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A50" s="30">
         <v>5.5146000000000001E-2</v>
       </c>
@@ -18240,7 +18256,7 @@
         <v>-1.9935000000000001E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:36">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51" s="30">
         <v>5.4336000000000002E-2</v>
       </c>
@@ -18350,7 +18366,7 @@
         <v>-1.9289000000000001E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:36">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52" s="30">
         <v>5.3359999999999998E-2</v>
       </c>
@@ -18460,7 +18476,7 @@
         <v>-1.8554999999999999E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:36">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53" s="30">
         <v>5.2211E-2</v>
       </c>
@@ -18570,7 +18586,7 @@
         <v>-1.8151E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:36">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54" s="30">
         <v>5.0758999999999999E-2</v>
       </c>
@@ -18680,7 +18696,7 @@
         <v>-1.7795999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:36">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55" s="30">
         <v>4.9699E-2</v>
       </c>
@@ -18790,7 +18806,7 @@
         <v>-1.7281000000000001E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:36">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56" s="30">
         <v>4.9028000000000002E-2</v>
       </c>
@@ -18900,7 +18916,7 @@
         <v>-1.6966999999999999E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:36">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57" s="30">
         <v>4.8057000000000002E-2</v>
       </c>
@@ -19010,7 +19026,7 @@
         <v>-1.6674999999999999E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:36">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58" s="30">
         <v>4.7393999999999999E-2</v>
       </c>
@@ -19120,7 +19136,7 @@
         <v>-1.6372000000000001E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:36">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A59" s="30">
         <v>4.6948999999999998E-2</v>
       </c>
@@ -19230,7 +19246,7 @@
         <v>-1.6211E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:36">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A60" s="30">
         <v>4.6358000000000003E-2</v>
       </c>
@@ -19340,7 +19356,7 @@
         <v>-1.5982E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:36">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61" s="30">
         <v>4.6005999999999998E-2</v>
       </c>
@@ -19450,7 +19466,7 @@
         <v>-1.5730999999999998E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:36">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A62" s="30">
         <v>4.5657000000000003E-2</v>
       </c>
@@ -19560,7 +19576,7 @@
         <v>-1.5650000000000001E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:36">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63" s="30">
         <v>4.4887999999999997E-2</v>
       </c>
@@ -19670,7 +19686,7 @@
         <v>-1.5442000000000001E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:36">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64" s="30">
         <v>4.4344000000000001E-2</v>
       </c>
@@ -19780,7 +19796,7 @@
         <v>-1.5474999999999999E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:36">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A65" s="30">
         <v>4.3698000000000001E-2</v>
       </c>
@@ -19890,7 +19906,7 @@
         <v>-1.5446E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:36">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A66" s="30">
         <v>4.2992000000000002E-2</v>
       </c>
@@ -20000,7 +20016,7 @@
         <v>-1.5382E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:36">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A67" s="30">
         <v>4.2221000000000002E-2</v>
       </c>
@@ -20110,7 +20126,7 @@
         <v>-1.5272000000000001E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:36">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A68" s="30">
         <v>4.2258999999999998E-2</v>
       </c>
@@ -20220,7 +20236,7 @@
         <v>-1.5022000000000001E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:36">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A69" s="30">
         <v>4.1813000000000003E-2</v>
       </c>
@@ -20330,7 +20346,7 @@
         <v>-1.4598E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:36">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A70" s="30">
         <v>4.1190999999999998E-2</v>
       </c>
@@ -20440,7 +20456,7 @@
         <v>-1.439E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:36">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A71" s="30">
         <v>4.1315999999999999E-2</v>
       </c>
@@ -20550,7 +20566,7 @@
         <v>-1.4239E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:36">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A72" s="30">
         <v>4.0593999999999998E-2</v>
       </c>
@@ -20660,7 +20676,7 @@
         <v>-1.4161E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:36">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A73" s="30">
         <v>4.0902000000000001E-2</v>
       </c>
@@ -20770,7 +20786,7 @@
         <v>-1.4272999999999999E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:36">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A74" s="30">
         <v>4.0507000000000001E-2</v>
       </c>
@@ -20880,7 +20896,7 @@
         <v>-1.4279999999999999E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:36">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A75" s="30">
         <v>4.1043999999999997E-2</v>
       </c>
@@ -20990,7 +21006,7 @@
         <v>-1.4352999999999999E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:36">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A76" s="30">
         <v>4.0555000000000001E-2</v>
       </c>
@@ -21100,7 +21116,7 @@
         <v>-1.4429000000000001E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:36">
+    <row r="77" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A77" s="30">
         <v>4.1255E-2</v>
       </c>
@@ -21210,7 +21226,7 @@
         <v>-1.4637000000000001E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:36">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A78" s="30">
         <v>4.0912999999999998E-2</v>
       </c>
@@ -21320,7 +21336,7 @@
         <v>-1.4713E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:36">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A79" s="30">
         <v>4.1392999999999999E-2</v>
       </c>
@@ -21430,7 +21446,7 @@
         <v>-1.5044E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:36">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A80" s="30">
         <v>4.0951000000000001E-2</v>
       </c>
@@ -21540,7 +21556,7 @@
         <v>-1.5200999999999999E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:36">
+    <row r="81" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A81" s="30">
         <v>4.0934999999999999E-2</v>
       </c>
@@ -21650,7 +21666,7 @@
         <v>-1.54E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:36">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A82" s="30">
         <v>4.0092999999999997E-2</v>
       </c>
@@ -21760,7 +21776,7 @@
         <v>-1.5492000000000001E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:36">
+    <row r="83" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A83" s="30">
         <v>3.9625E-2</v>
       </c>
@@ -21870,7 +21886,7 @@
         <v>-1.5389E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:36">
+    <row r="84" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A84" s="30">
         <v>3.8066000000000003E-2</v>
       </c>
@@ -21980,7 +21996,7 @@
         <v>-1.4987E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:36">
+    <row r="85" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A85" s="30">
         <v>3.8646E-2</v>
       </c>

</xml_diff>